<commit_message>
Require Python 3.7 or newer We don't require pymodbus
</commit_message>
<xml_diff>
--- a/docs/RegisterNames_pyflexit.xlsx
+++ b/docs/RegisterNames_pyflexit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyma\GitHub\pyflexit\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marhoy/GitHub/pyflexit/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BF430D-7923-48CF-99B6-8663FBCA36B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438059E4-A47E-4043-9ABC-6A238DDD62C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="612" yWindow="2004" windowWidth="29856" windowHeight="11988" xr2:uid="{FF5E6A59-2A44-4AE2-B875-90AAE0108086}"/>
+    <workbookView xWindow="0" yWindow="3620" windowWidth="28800" windowHeight="16840" xr2:uid="{FF5E6A59-2A44-4AE2-B875-90AAE0108086}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="59">
   <si>
     <t>Modbus
 address</t>
@@ -177,23 +177,47 @@
     <t>Filter</t>
   </si>
   <si>
-    <t>Temperatures</t>
-  </si>
-  <si>
     <t>Heating</t>
   </si>
   <si>
-    <t>Fan mode</t>
-  </si>
-  <si>
-    <t>ElectricHeaterPowerSupplyAir</t>
+    <t>ExhaustFanSpeed</t>
+  </si>
+  <si>
+    <t>SupplyFanSpeed</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>RoomHumidity1</t>
+  </si>
+  <si>
+    <t>RoomHumidity2</t>
+  </si>
+  <si>
+    <t>RoomHumidity3</t>
+  </si>
+  <si>
+    <t>ElectricHeaterPower</t>
+  </si>
+  <si>
+    <t>RoomAirQuality1</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>Room Sensors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,13 +293,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,37 +342,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -667,31 +686,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADB44AE-C7DA-4920-BAF1-9DECDE18635E}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="32.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="8" width="8.88671875" style="17"/>
-    <col min="9" max="9" width="18.44140625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="1"/>
-    <col min="13" max="13" width="8.88671875" style="4"/>
-    <col min="14" max="14" width="8.88671875" style="12"/>
-    <col min="15" max="15" width="18.44140625" style="18" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="17"/>
+    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="8" width="8.83203125" style="16"/>
+    <col min="9" max="9" width="18.5" style="23" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="1"/>
+    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="3"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="18.5" style="17" customWidth="1"/>
+    <col min="20" max="20" width="8.83203125" style="16"/>
     <col min="21" max="21" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32"/>
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="18" thickBot="1">
+      <c r="A1" s="27"/>
       <c r="E1" s="30" t="s">
         <v>6</v>
       </c>
@@ -714,215 +734,221 @@
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
     </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:21" s="6" customFormat="1" ht="34" thickTop="1" thickBot="1">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="U2" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:21" s="22" customFormat="1" ht="16">
+      <c r="A3" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="K3" s="25">
+      <c r="G3" s="23"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="K3" s="22">
         <v>1163</v>
       </c>
-      <c r="L3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="29" t="s">
+      <c r="L3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="Q3" s="25">
+      <c r="O3" s="26"/>
+      <c r="Q3" s="27">
         <v>1163</v>
       </c>
-      <c r="R3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="29" t="s">
+      <c r="R3" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="8" t="s">
+      <c r="U3" s="26"/>
+    </row>
+    <row r="4" spans="1:21" ht="16">
+      <c r="A4" s="29"/>
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="29"/>
+      <c r="F4" s="15"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="26"/>
       <c r="K4">
         <v>1155</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="15" t="s">
+      <c r="M4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="Q4" s="3">
+      <c r="O4" s="19"/>
+      <c r="Q4" s="27">
         <v>1155</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="T4" s="15" t="s">
+      <c r="R4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="8" t="s">
+      <c r="U4" s="26"/>
+    </row>
+    <row r="5" spans="1:21" s="15" customFormat="1" ht="16">
+      <c r="A5" s="29"/>
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="16">
-        <v>9</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="E5" s="15">
+        <v>9</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="20"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="15"/>
-    </row>
-    <row r="6" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="9" t="s">
+      <c r="I5" s="26"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="19"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+    </row>
+    <row r="6" spans="1:21" s="10" customFormat="1" ht="16">
+      <c r="A6" s="29"/>
+      <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>12</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="K6" s="11">
+      <c r="I6" s="26"/>
+      <c r="K6" s="10">
         <v>1</v>
       </c>
-      <c r="L6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="15" t="s">
+      <c r="L6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="20"/>
-      <c r="Q6" s="16">
+      <c r="O6" s="19"/>
+      <c r="Q6" s="27">
         <v>1</v>
       </c>
-      <c r="R6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" s="15" t="s">
+      <c r="R6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="9" t="s">
+      <c r="U6" s="26"/>
+    </row>
+    <row r="7" spans="1:21" ht="16">
+      <c r="A7" s="29"/>
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="1">
@@ -931,61 +957,62 @@
       <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="26"/>
       <c r="K7">
         <v>5</v>
       </c>
       <c r="L7" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" s="15" t="s">
+      <c r="M7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="20"/>
-      <c r="Q7" s="16">
+      <c r="O7" s="19"/>
+      <c r="Q7" s="27">
         <v>5</v>
       </c>
-      <c r="R7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="S7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="T7" s="15" t="s">
+      <c r="R7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="9" t="s">
+      <c r="U7" s="26"/>
+    </row>
+    <row r="8" spans="1:21" s="10" customFormat="1" ht="16">
+      <c r="A8" s="29"/>
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1">
         <v>11</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="17" t="s">
+      <c r="F8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="26"/>
       <c r="J8" s="1"/>
       <c r="K8">
         <v>9</v>
@@ -993,70 +1020,72 @@
       <c r="L8" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="15" t="s">
+      <c r="M8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="Q8" s="16">
-        <v>9</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="T8" s="15" t="s">
+      <c r="O8" s="19"/>
+      <c r="Q8" s="27">
+        <v>9</v>
+      </c>
+      <c r="R8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T8" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="9" t="s">
+      <c r="U8" s="26"/>
+    </row>
+    <row r="9" spans="1:21" ht="16">
+      <c r="A9" s="29"/>
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="29"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="26"/>
       <c r="K9">
         <v>13</v>
       </c>
       <c r="L9" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9" s="15" t="s">
+      <c r="M9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="Q9" s="16">
+      <c r="O9" s="19"/>
+      <c r="Q9" s="27">
         <v>13</v>
       </c>
-      <c r="R9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="T9" s="15" t="s">
+      <c r="R9" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="U9" s="26"/>
+    </row>
+    <row r="10" spans="1:21" ht="16">
+      <c r="A10" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="1">
@@ -1065,10 +1094,10 @@
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K10">
@@ -1077,32 +1106,32 @@
       <c r="L10" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O10" s="23" t="s">
+      <c r="O10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="27">
         <v>3034</v>
       </c>
-      <c r="R10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10" s="22" t="s">
+      <c r="R10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T10" s="22"/>
-      <c r="U10" s="23" t="s">
+      <c r="T10" s="28"/>
+      <c r="U10" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="1:21" ht="16">
+      <c r="A11" s="29"/>
+      <c r="B11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="21" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="1">
@@ -1111,10 +1140,10 @@
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K11">
@@ -1123,211 +1152,419 @@
       <c r="L11" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O11" s="23" t="s">
+      <c r="O11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="25">
+      <c r="Q11" s="27">
         <v>2013</v>
       </c>
-      <c r="R11" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="S11" s="26" t="s">
+      <c r="R11" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T11" s="26"/>
-      <c r="U11" s="23" t="s">
+      <c r="T11" s="28"/>
+      <c r="U11" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:21" s="27" customFormat="1">
+      <c r="A12" s="29"/>
+      <c r="B12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="21"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="20"/>
+      <c r="K12" s="27">
+        <v>9</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="20"/>
+      <c r="Q12" s="27">
+        <v>9</v>
+      </c>
+      <c r="R12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U12" s="20"/>
+    </row>
+    <row r="13" spans="1:21" s="27" customFormat="1">
+      <c r="A13" s="29"/>
+      <c r="B13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="27">
+        <v>5</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="Q13" s="27">
+        <v>5</v>
+      </c>
+      <c r="R13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T13" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U13" s="20"/>
+    </row>
+    <row r="14" spans="1:21" s="27" customFormat="1" ht="16">
+      <c r="A14" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C14" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E14" s="27">
         <v>15</v>
       </c>
-      <c r="F12" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="33" t="s">
+      <c r="F14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H14" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="33"/>
-      <c r="K12" s="32">
+      <c r="I14" s="28"/>
+      <c r="K14" s="27">
         <v>1</v>
       </c>
-      <c r="L12" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12" s="33" t="s">
+      <c r="L14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="33"/>
-      <c r="Q12" s="32">
+      <c r="O14" s="28"/>
+      <c r="Q14" s="27">
         <v>1</v>
       </c>
-      <c r="R12" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="S12" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="T12" s="33" t="s">
+      <c r="R14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T14" s="28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="U14" s="28"/>
+    </row>
+    <row r="15" spans="1:21" s="27" customFormat="1" ht="16">
+      <c r="A15" s="29"/>
+      <c r="B15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E15" s="27">
         <v>16</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="33" t="s">
+      <c r="F15" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H15" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="K13" s="32">
+      <c r="I15" s="28"/>
+      <c r="K15" s="27">
         <v>13</v>
       </c>
-      <c r="L13" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13" s="33" t="s">
+      <c r="L15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="O13" s="33"/>
-      <c r="Q13" s="32">
+      <c r="O15" s="28"/>
+      <c r="Q15" s="27">
         <v>13</v>
       </c>
-      <c r="R13" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="S13" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="T13" s="33" t="s">
+      <c r="R15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" s="28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="U15" s="28"/>
+    </row>
+    <row r="16" spans="1:21" ht="16">
+      <c r="A16" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="1">
-        <v>9</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="17" t="s">
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K14">
+      <c r="K16">
         <v>1271</v>
       </c>
-      <c r="L14" t="s">
-        <v>7</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14" s="12" t="s">
+      <c r="L16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q16" s="27">
         <v>1271</v>
       </c>
-      <c r="R14" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="S14" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="T14" s="26" t="s">
+      <c r="R16" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T16" s="28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="9" t="s">
+      <c r="U16" s="28"/>
+    </row>
+    <row r="17" spans="1:21" ht="16">
+      <c r="A17" s="29"/>
+      <c r="B17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C17" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="K15">
+      <c r="K17">
         <v>1269</v>
       </c>
-      <c r="L15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="12" t="s">
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q17" s="27">
         <v>1269</v>
       </c>
-      <c r="R15" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="S15" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="T15" s="26" t="s">
+      <c r="R17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S17" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T17" s="28" t="s">
         <v>23</v>
       </c>
+      <c r="U17" s="28"/>
+    </row>
+    <row r="18" spans="1:21" s="27" customFormat="1">
+      <c r="A18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="K18" s="27">
+        <v>1007</v>
+      </c>
+      <c r="L18" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="O18" s="28"/>
+      <c r="Q18" s="27">
+        <v>1007</v>
+      </c>
+      <c r="R18" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S18" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="U18" s="28"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="29"/>
+      <c r="B19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19">
+        <v>1001</v>
+      </c>
+      <c r="L19" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q19" s="27">
+        <v>1001</v>
+      </c>
+      <c r="R19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S19" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T19" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U19" s="28"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="29"/>
+      <c r="B20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" s="27">
+        <v>1003</v>
+      </c>
+      <c r="L20" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="27">
+        <v>1003</v>
+      </c>
+      <c r="R20" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S20" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U20" s="28"/>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="29"/>
+      <c r="B21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="27">
+        <v>1005</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q21" s="27">
+        <v>1005</v>
+      </c>
+      <c r="R21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="T21" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U21" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E1:I1"/>
+  <mergeCells count="8">
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="E1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>